<commit_message>
finished and tested with TomoKISStudio and with simulator
</commit_message>
<xml_diff>
--- a/FilteredElectrodesPairs.xlsx
+++ b/FilteredElectrodesPairs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekty\RocsoleDataConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677370FB-37F7-4753-A18B-4931F0D022CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3F3842-11B1-42AF-9EE1-CE5AE6F336E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="16176" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="29460" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Normalized" sheetId="1" r:id="rId1"/>
+    <sheet name="RAW" sheetId="2" r:id="rId1"/>
+    <sheet name="Normalized" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>LiczbaElektrod</t>
   </si>
@@ -102,13 +103,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +391,1952 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F37C97E-4A92-48F8-8517-257DD2D99655}">
+  <dimension ref="A1:N129"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <f>M2/2</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
+        <f>M2/2</f>
+        <v>8</v>
+      </c>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="L7" s="5">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2">
+        <f>IF(L6&gt;=$M$3,"",M6+$M$2+1)</f>
+        <v>25</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="L8" s="5">
+        <v>3</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" ref="M8:M26" si="0">IF(L7&gt;=$M$3,"",M7+$M$2+1)</f>
+        <v>42</v>
+      </c>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="L9" s="5">
+        <v>4</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>9</v>
+      </c>
+      <c r="H10" s="6">
+        <v>8</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="L10" s="5">
+        <v>5</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
+      <c r="L11" s="5">
+        <v>6</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="L12" s="5">
+        <v>7</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="L13" s="5">
+        <v>8</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>9</v>
+      </c>
+      <c r="M14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>2</v>
+      </c>
+      <c r="B15" s="6">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>13</v>
+      </c>
+      <c r="D15" s="6">
+        <f>C15-C6</f>
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="M15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="L16">
+        <v>11</v>
+      </c>
+      <c r="M16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+      <c r="L17">
+        <v>12</v>
+      </c>
+      <c r="M17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="L18">
+        <v>13</v>
+      </c>
+      <c r="M18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>17</v>
+      </c>
+      <c r="L19">
+        <v>14</v>
+      </c>
+      <c r="M19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="L20">
+        <v>15</v>
+      </c>
+      <c r="M20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>19</v>
+      </c>
+      <c r="L21">
+        <v>16</v>
+      </c>
+      <c r="M21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>20</v>
+      </c>
+      <c r="L22">
+        <v>17</v>
+      </c>
+      <c r="M22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>21</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>21</v>
+      </c>
+      <c r="L23">
+        <v>18</v>
+      </c>
+      <c r="M23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>3</v>
+      </c>
+      <c r="B24" s="6">
+        <v>7</v>
+      </c>
+      <c r="C24" s="6">
+        <v>22</v>
+      </c>
+      <c r="D24" s="6">
+        <f>C24-C15</f>
+        <v>9</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>22</v>
+      </c>
+      <c r="L24">
+        <v>19</v>
+      </c>
+      <c r="M24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <v>23</v>
+      </c>
+      <c r="L25">
+        <v>20</v>
+      </c>
+      <c r="M25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>24</v>
+      </c>
+      <c r="L26">
+        <v>21</v>
+      </c>
+      <c r="M26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="F27" s="6">
+        <v>2</v>
+      </c>
+      <c r="G27" s="6">
+        <v>10</v>
+      </c>
+      <c r="H27" s="6">
+        <v>25</v>
+      </c>
+      <c r="I27" s="6">
+        <f>H27-H10</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>11</v>
+      </c>
+      <c r="H28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>12</v>
+      </c>
+      <c r="H29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>28</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>13</v>
+      </c>
+      <c r="H30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>14</v>
+      </c>
+      <c r="H31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>15</v>
+      </c>
+      <c r="H32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="6">
+        <v>4</v>
+      </c>
+      <c r="B33" s="6">
+        <v>8</v>
+      </c>
+      <c r="C33" s="6">
+        <v>31</v>
+      </c>
+      <c r="D33" s="6">
+        <f>C33-C24</f>
+        <v>9</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>16</v>
+      </c>
+      <c r="H33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F39">
+        <v>3</v>
+      </c>
+      <c r="G39">
+        <v>6</v>
+      </c>
+      <c r="H39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>8</v>
+      </c>
+      <c r="H41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <v>10</v>
+      </c>
+      <c r="H43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F44" s="6">
+        <v>3</v>
+      </c>
+      <c r="G44" s="6">
+        <v>11</v>
+      </c>
+      <c r="H44" s="6">
+        <v>42</v>
+      </c>
+      <c r="I44" s="6">
+        <f>H44-H27</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>12</v>
+      </c>
+      <c r="H45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>13</v>
+      </c>
+      <c r="H46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>14</v>
+      </c>
+      <c r="H47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>15</v>
+      </c>
+      <c r="H48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <v>3</v>
+      </c>
+      <c r="G49">
+        <v>16</v>
+      </c>
+      <c r="H49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F50">
+        <v>4</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <v>4</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <v>4</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
+      <c r="H54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <v>4</v>
+      </c>
+      <c r="G55">
+        <v>6</v>
+      </c>
+      <c r="H55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F56">
+        <v>4</v>
+      </c>
+      <c r="G56">
+        <v>7</v>
+      </c>
+      <c r="H56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F57">
+        <v>4</v>
+      </c>
+      <c r="G57">
+        <v>8</v>
+      </c>
+      <c r="H57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F58">
+        <v>4</v>
+      </c>
+      <c r="G58">
+        <v>9</v>
+      </c>
+      <c r="H58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <v>4</v>
+      </c>
+      <c r="G59">
+        <v>10</v>
+      </c>
+      <c r="H59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F60">
+        <v>4</v>
+      </c>
+      <c r="G60">
+        <v>11</v>
+      </c>
+      <c r="H60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F61" s="6">
+        <v>4</v>
+      </c>
+      <c r="G61" s="6">
+        <v>12</v>
+      </c>
+      <c r="H61" s="6">
+        <v>59</v>
+      </c>
+      <c r="I61" s="6">
+        <f>H61-H44</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F62">
+        <v>4</v>
+      </c>
+      <c r="G62">
+        <v>13</v>
+      </c>
+      <c r="H62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F63">
+        <v>4</v>
+      </c>
+      <c r="G63">
+        <v>14</v>
+      </c>
+      <c r="H63">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F64">
+        <v>4</v>
+      </c>
+      <c r="G64">
+        <v>15</v>
+      </c>
+      <c r="H64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F65">
+        <v>4</v>
+      </c>
+      <c r="G65">
+        <v>16</v>
+      </c>
+      <c r="H65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F66">
+        <v>5</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F67">
+        <v>5</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F68">
+        <v>5</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F69">
+        <v>5</v>
+      </c>
+      <c r="G69">
+        <v>4</v>
+      </c>
+      <c r="H69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F70">
+        <v>5</v>
+      </c>
+      <c r="G70">
+        <v>5</v>
+      </c>
+      <c r="H70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F71">
+        <v>5</v>
+      </c>
+      <c r="G71">
+        <v>6</v>
+      </c>
+      <c r="H71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F72">
+        <v>5</v>
+      </c>
+      <c r="G72">
+        <v>7</v>
+      </c>
+      <c r="H72">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <v>5</v>
+      </c>
+      <c r="G73">
+        <v>8</v>
+      </c>
+      <c r="H73">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F74">
+        <v>5</v>
+      </c>
+      <c r="G74">
+        <v>9</v>
+      </c>
+      <c r="H74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <v>5</v>
+      </c>
+      <c r="G75">
+        <v>10</v>
+      </c>
+      <c r="H75">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F76">
+        <v>5</v>
+      </c>
+      <c r="G76">
+        <v>11</v>
+      </c>
+      <c r="H76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F77">
+        <v>5</v>
+      </c>
+      <c r="G77">
+        <v>12</v>
+      </c>
+      <c r="H77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F78" s="6">
+        <v>5</v>
+      </c>
+      <c r="G78" s="6">
+        <v>13</v>
+      </c>
+      <c r="H78" s="6">
+        <v>76</v>
+      </c>
+      <c r="I78" s="6">
+        <f>H78-H61</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F79">
+        <v>5</v>
+      </c>
+      <c r="G79">
+        <v>14</v>
+      </c>
+      <c r="H79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F80">
+        <v>5</v>
+      </c>
+      <c r="G80">
+        <v>15</v>
+      </c>
+      <c r="H80">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F81">
+        <v>5</v>
+      </c>
+      <c r="G81">
+        <v>16</v>
+      </c>
+      <c r="H81">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <v>6</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F83">
+        <v>6</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+      <c r="H83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F84">
+        <v>6</v>
+      </c>
+      <c r="G84">
+        <v>3</v>
+      </c>
+      <c r="H84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F85">
+        <v>6</v>
+      </c>
+      <c r="G85">
+        <v>4</v>
+      </c>
+      <c r="H85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F86">
+        <v>6</v>
+      </c>
+      <c r="G86">
+        <v>5</v>
+      </c>
+      <c r="H86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F87">
+        <v>6</v>
+      </c>
+      <c r="G87">
+        <v>6</v>
+      </c>
+      <c r="H87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F88">
+        <v>6</v>
+      </c>
+      <c r="G88">
+        <v>7</v>
+      </c>
+      <c r="H88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F89">
+        <v>6</v>
+      </c>
+      <c r="G89">
+        <v>8</v>
+      </c>
+      <c r="H89">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F90">
+        <v>6</v>
+      </c>
+      <c r="G90">
+        <v>9</v>
+      </c>
+      <c r="H90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F91">
+        <v>6</v>
+      </c>
+      <c r="G91">
+        <v>10</v>
+      </c>
+      <c r="H91">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F92">
+        <v>6</v>
+      </c>
+      <c r="G92">
+        <v>11</v>
+      </c>
+      <c r="H92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F93">
+        <v>6</v>
+      </c>
+      <c r="G93">
+        <v>12</v>
+      </c>
+      <c r="H93">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F94">
+        <v>6</v>
+      </c>
+      <c r="G94">
+        <v>13</v>
+      </c>
+      <c r="H94">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F95" s="6">
+        <v>6</v>
+      </c>
+      <c r="G95" s="6">
+        <v>14</v>
+      </c>
+      <c r="H95" s="6">
+        <v>93</v>
+      </c>
+      <c r="I95" s="6">
+        <f>H95-H78</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F96">
+        <v>6</v>
+      </c>
+      <c r="G96">
+        <v>15</v>
+      </c>
+      <c r="H96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F97">
+        <v>6</v>
+      </c>
+      <c r="G97">
+        <v>16</v>
+      </c>
+      <c r="H97">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F98">
+        <v>7</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F99">
+        <v>7</v>
+      </c>
+      <c r="G99">
+        <v>2</v>
+      </c>
+      <c r="H99">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F100">
+        <v>7</v>
+      </c>
+      <c r="G100">
+        <v>3</v>
+      </c>
+      <c r="H100">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F101">
+        <v>7</v>
+      </c>
+      <c r="G101">
+        <v>4</v>
+      </c>
+      <c r="H101">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F102">
+        <v>7</v>
+      </c>
+      <c r="G102">
+        <v>5</v>
+      </c>
+      <c r="H102">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F103">
+        <v>7</v>
+      </c>
+      <c r="G103">
+        <v>6</v>
+      </c>
+      <c r="H103">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F104">
+        <v>7</v>
+      </c>
+      <c r="G104">
+        <v>7</v>
+      </c>
+      <c r="H104">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F105">
+        <v>7</v>
+      </c>
+      <c r="G105">
+        <v>8</v>
+      </c>
+      <c r="H105">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F106">
+        <v>7</v>
+      </c>
+      <c r="G106">
+        <v>9</v>
+      </c>
+      <c r="H106">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F107">
+        <v>7</v>
+      </c>
+      <c r="G107">
+        <v>10</v>
+      </c>
+      <c r="H107">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F108">
+        <v>7</v>
+      </c>
+      <c r="G108">
+        <v>11</v>
+      </c>
+      <c r="H108">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F109">
+        <v>7</v>
+      </c>
+      <c r="G109">
+        <v>12</v>
+      </c>
+      <c r="H109">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F110">
+        <v>7</v>
+      </c>
+      <c r="G110">
+        <v>13</v>
+      </c>
+      <c r="H110">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F111">
+        <v>7</v>
+      </c>
+      <c r="G111">
+        <v>14</v>
+      </c>
+      <c r="H111">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F112" s="6">
+        <v>7</v>
+      </c>
+      <c r="G112" s="6">
+        <v>15</v>
+      </c>
+      <c r="H112" s="6">
+        <v>110</v>
+      </c>
+      <c r="I112" s="6">
+        <f>H112-H95</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="113" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F113">
+        <v>7</v>
+      </c>
+      <c r="G113">
+        <v>16</v>
+      </c>
+      <c r="H113">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F114">
+        <v>8</v>
+      </c>
+      <c r="G114">
+        <v>1</v>
+      </c>
+      <c r="H114">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F115">
+        <v>8</v>
+      </c>
+      <c r="G115">
+        <v>2</v>
+      </c>
+      <c r="H115">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F116">
+        <v>8</v>
+      </c>
+      <c r="G116">
+        <v>3</v>
+      </c>
+      <c r="H116">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F117">
+        <v>8</v>
+      </c>
+      <c r="G117">
+        <v>4</v>
+      </c>
+      <c r="H117">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F118">
+        <v>8</v>
+      </c>
+      <c r="G118">
+        <v>5</v>
+      </c>
+      <c r="H118">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F119">
+        <v>8</v>
+      </c>
+      <c r="G119">
+        <v>6</v>
+      </c>
+      <c r="H119">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F120">
+        <v>8</v>
+      </c>
+      <c r="G120">
+        <v>7</v>
+      </c>
+      <c r="H120">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F121">
+        <v>8</v>
+      </c>
+      <c r="G121">
+        <v>8</v>
+      </c>
+      <c r="H121">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F122">
+        <v>8</v>
+      </c>
+      <c r="G122">
+        <v>9</v>
+      </c>
+      <c r="H122">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="123" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F123">
+        <v>8</v>
+      </c>
+      <c r="G123">
+        <v>10</v>
+      </c>
+      <c r="H123">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="124" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F124">
+        <v>8</v>
+      </c>
+      <c r="G124">
+        <v>11</v>
+      </c>
+      <c r="H124">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F125">
+        <v>8</v>
+      </c>
+      <c r="G125">
+        <v>12</v>
+      </c>
+      <c r="H125">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F126">
+        <v>8</v>
+      </c>
+      <c r="G126">
+        <v>13</v>
+      </c>
+      <c r="H126">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="127" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F127">
+        <v>8</v>
+      </c>
+      <c r="G127">
+        <v>14</v>
+      </c>
+      <c r="H127">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="128" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F128">
+        <v>8</v>
+      </c>
+      <c r="G128">
+        <v>15</v>
+      </c>
+      <c r="H128">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="129" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="F129" s="6">
+        <v>8</v>
+      </c>
+      <c r="G129" s="6">
+        <v>16</v>
+      </c>
+      <c r="H129" s="6">
+        <v>127</v>
+      </c>
+      <c r="I129" s="6">
+        <f>H129-H112</f>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -418,7 +2363,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -427,7 +2372,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="s">
         <v>0</v>
@@ -444,7 +2389,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -453,7 +2398,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3" t="s">
         <v>1</v>
@@ -475,7 +2420,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
@@ -484,7 +2429,7 @@
         <v>4</v>
       </c>
       <c r="I4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -495,7 +2440,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -504,7 +2449,7 @@
         <v>5</v>
       </c>
       <c r="I5" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J5" s="3"/>
     </row>
@@ -516,7 +2461,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -525,18 +2470,18 @@
         <v>6</v>
       </c>
       <c r="I6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
       <c r="N6" s="4">
-        <f>N2/2</f>
-        <v>8</v>
+        <f>N2/2-1</f>
+        <v>7</v>
       </c>
       <c r="O6" s="2">
         <f>N6-1</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -547,7 +2492,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1">
         <v>1</v>
@@ -556,18 +2501,18 @@
         <v>7</v>
       </c>
       <c r="I7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M7" s="5">
         <v>2</v>
       </c>
       <c r="N7" s="3">
-        <f>IF(M6&gt;=$N$3,"",N6+$N$2-M6)</f>
-        <v>23</v>
+        <f t="shared" ref="N7:N26" si="0">IF(M6&gt;=$N$3,"",N6+$N$2-M6)</f>
+        <v>22</v>
       </c>
       <c r="O7" s="2">
         <f>IF(M6&gt;=$N$3,"",N7-1)</f>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -578,7 +2523,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
@@ -587,18 +2532,18 @@
         <v>8</v>
       </c>
       <c r="I8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M8" s="5">
         <v>3</v>
       </c>
       <c r="N8" s="3">
-        <f>IF(M7&gt;=$N$3,"",N7+$N$2-M7)</f>
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="O8" s="2">
-        <f t="shared" ref="O8:O26" si="0">IF(M7&gt;=$N$3,"",N8-1)</f>
-        <v>36</v>
+        <f t="shared" ref="O8:O26" si="1">IF(M7&gt;=$N$3,"",N8-1)</f>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -609,7 +2554,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3"/>
       <c r="G9" s="1">
@@ -619,19 +2564,19 @@
         <v>3</v>
       </c>
       <c r="I9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M9" s="5">
         <v>4</v>
       </c>
       <c r="N9" s="3">
-        <f>IF(M8&gt;=$N$3,"",N8+$N$2-M8)</f>
-        <v>50</v>
-      </c>
-      <c r="O9" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
+      <c r="O9" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -641,7 +2586,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="1">
         <v>2</v>
@@ -650,19 +2595,19 @@
         <v>4</v>
       </c>
       <c r="I10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M10" s="5">
         <v>5</v>
       </c>
       <c r="N10" s="3">
-        <f>IF(M9&gt;=$N$3,"",N9+$N$2-M9)</f>
-        <v>62</v>
-      </c>
-      <c r="O10" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
+      <c r="O10" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -672,7 +2617,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" s="1">
         <v>2</v>
@@ -681,19 +2626,19 @@
         <v>5</v>
       </c>
       <c r="I11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M11" s="5">
         <v>6</v>
       </c>
       <c r="N11" s="3">
-        <f>IF(M10&gt;=$N$3,"",N10+$N$2-M10)</f>
-        <v>73</v>
-      </c>
-      <c r="O11" s="2">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
+      <c r="O11" s="2">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -703,7 +2648,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="3">
         <v>2</v>
@@ -712,7 +2657,7 @@
         <v>6</v>
       </c>
       <c r="I12" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J12" s="3">
         <f>I12-I5</f>
@@ -722,13 +2667,13 @@
         <v>7</v>
       </c>
       <c r="N12" s="3">
-        <f>IF(M11&gt;=$N$3,"",N11+$N$2-M11)</f>
-        <v>83</v>
-      </c>
-      <c r="O12" s="2">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
+      <c r="O12" s="2">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -738,7 +2683,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" s="1">
         <v>2</v>
@@ -747,19 +2692,19 @@
         <v>7</v>
       </c>
       <c r="I13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M13" s="5">
         <v>8</v>
       </c>
       <c r="N13" s="3">
-        <f>IF(M12&gt;=$N$3,"",N12+$N$2-M12)</f>
-        <v>92</v>
-      </c>
-      <c r="O13" s="2">
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
+      <c r="O13" s="2">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -769,7 +2714,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" s="1">
         <v>2</v>
@@ -778,19 +2723,19 @@
         <v>8</v>
       </c>
       <c r="I14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M14">
         <v>9</v>
       </c>
       <c r="N14" s="3" t="str">
-        <f>IF(M13&gt;=$N$3,"",N13+$N$2-M13)</f>
-        <v/>
-      </c>
-      <c r="O14" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -800,7 +2745,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="1">
         <v>3</v>
@@ -809,19 +2754,19 @@
         <v>4</v>
       </c>
       <c r="I15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M15">
         <v>10</v>
       </c>
       <c r="N15" s="3" t="str">
-        <f>IF(M14&gt;=$N$3,"",N14+$N$2-M14)</f>
-        <v/>
-      </c>
-      <c r="O15" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -831,7 +2776,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1">
         <v>3</v>
@@ -840,19 +2785,19 @@
         <v>5</v>
       </c>
       <c r="I16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M16">
         <v>11</v>
       </c>
       <c r="N16" s="3" t="str">
-        <f>IF(M15&gt;=$N$3,"",N15+$N$2-M15)</f>
-        <v/>
-      </c>
-      <c r="O16" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O16" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -862,7 +2807,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="1">
         <v>3</v>
@@ -871,19 +2816,19 @@
         <v>6</v>
       </c>
       <c r="I17" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M17">
         <v>12</v>
       </c>
       <c r="N17" s="3" t="str">
-        <f>IF(M16&gt;=$N$3,"",N16+$N$2-M16)</f>
-        <v/>
-      </c>
-      <c r="O17" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -893,7 +2838,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" s="3">
         <v>3</v>
@@ -902,7 +2847,7 @@
         <v>7</v>
       </c>
       <c r="I18" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J18" s="3">
         <f>I18-I12</f>
@@ -912,13 +2857,13 @@
         <v>13</v>
       </c>
       <c r="N18" s="3" t="str">
-        <f>IF(M17&gt;=$N$3,"",N17+$N$2-M17)</f>
-        <v/>
-      </c>
-      <c r="O18" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -928,7 +2873,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G19" s="1">
         <v>3</v>
@@ -937,19 +2882,19 @@
         <v>8</v>
       </c>
       <c r="I19" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M19">
         <v>14</v>
       </c>
       <c r="N19" s="3" t="str">
-        <f>IF(M18&gt;=$N$3,"",N18+$N$2-M18)</f>
-        <v/>
-      </c>
-      <c r="O19" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -959,7 +2904,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G20" s="1">
         <v>4</v>
@@ -968,19 +2913,19 @@
         <v>5</v>
       </c>
       <c r="I20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M20">
         <v>15</v>
       </c>
       <c r="N20" s="3" t="str">
-        <f>IF(M19&gt;=$N$3,"",N19+$N$2-M19)</f>
-        <v/>
-      </c>
-      <c r="O20" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -990,7 +2935,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G21" s="1">
         <v>4</v>
@@ -999,19 +2944,19 @@
         <v>6</v>
       </c>
       <c r="I21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M21">
         <v>16</v>
       </c>
       <c r="N21" s="3" t="str">
-        <f>IF(M20&gt;=$N$3,"",N20+$N$2-M20)</f>
-        <v/>
-      </c>
-      <c r="O21" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1021,7 +2966,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="1">
         <v>4</v>
@@ -1030,19 +2975,19 @@
         <v>7</v>
       </c>
       <c r="I22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M22">
         <v>17</v>
       </c>
       <c r="N22" s="3" t="str">
-        <f>IF(M21&gt;=$N$3,"",N21+$N$2-M21)</f>
-        <v/>
-      </c>
-      <c r="O22" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
@@ -1052,7 +2997,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1">
         <f>C23-C8</f>
@@ -1065,7 +3010,7 @@
         <v>8</v>
       </c>
       <c r="I23" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J23" s="3">
         <f>I23-I18</f>
@@ -1075,13 +3020,13 @@
         <v>18</v>
       </c>
       <c r="N23" s="3" t="str">
-        <f>IF(M22&gt;=$N$3,"",N22+$N$2-M22)</f>
-        <v/>
-      </c>
-      <c r="O23" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
@@ -1091,7 +3036,7 @@
         <v>10</v>
       </c>
       <c r="C24" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="3">
         <f>C24-C9</f>
@@ -1104,19 +3049,19 @@
         <v>6</v>
       </c>
       <c r="I24" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M24">
         <v>19</v>
       </c>
       <c r="N24" s="3" t="str">
-        <f>IF(M23&gt;=$N$3,"",N23+$N$2-M23)</f>
-        <v/>
-      </c>
-      <c r="O24" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -1126,7 +3071,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G25" s="1">
         <v>5</v>
@@ -1135,19 +3080,19 @@
         <v>7</v>
       </c>
       <c r="I25" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M25">
         <v>20</v>
       </c>
       <c r="N25" s="3" t="str">
-        <f>IF(M24&gt;=$N$3,"",N24+$N$2-M24)</f>
-        <v/>
-      </c>
-      <c r="O25" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -1157,7 +3102,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" s="1">
         <v>5</v>
@@ -1166,19 +3111,19 @@
         <v>8</v>
       </c>
       <c r="I26" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M26">
         <v>21</v>
       </c>
       <c r="N26" s="3" t="str">
-        <f>IF(M25&gt;=$N$3,"",N25+$N$2-M25)</f>
-        <v/>
-      </c>
-      <c r="O26" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="O26" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -1188,7 +3133,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27" s="1">
         <v>6</v>
@@ -1197,7 +3142,7 @@
         <v>7</v>
       </c>
       <c r="I27" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -1208,7 +3153,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" s="1">
         <v>6</v>
@@ -1217,7 +3162,7 @@
         <v>8</v>
       </c>
       <c r="I28" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -1228,7 +3173,7 @@
         <v>15</v>
       </c>
       <c r="C29" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G29" s="1">
         <v>7</v>
@@ -1237,7 +3182,7 @@
         <v>8</v>
       </c>
       <c r="I29" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -1248,7 +3193,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -1259,7 +3204,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -1270,7 +3215,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H32" s="3"/>
     </row>
@@ -1282,7 +3227,7 @@
         <v>6</v>
       </c>
       <c r="C33" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1293,7 +3238,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1304,7 +3249,7 @@
         <v>8</v>
       </c>
       <c r="C35" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H35" s="3"/>
     </row>
@@ -1316,7 +3261,7 @@
         <v>9</v>
       </c>
       <c r="C36" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1327,7 +3272,7 @@
         <v>10</v>
       </c>
       <c r="C37" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="1">
         <f>C37-C23</f>
@@ -1342,7 +3287,7 @@
         <v>11</v>
       </c>
       <c r="C38" s="3">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="3">
         <f>C38-C24</f>
@@ -1357,7 +3302,7 @@
         <v>12</v>
       </c>
       <c r="C39" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -1368,7 +3313,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -1379,7 +3324,7 @@
         <v>14</v>
       </c>
       <c r="C41" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -1390,7 +3335,7 @@
         <v>15</v>
       </c>
       <c r="C42" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -1401,7 +3346,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -1412,7 +3357,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -1423,7 +3368,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -1434,7 +3379,7 @@
         <v>7</v>
       </c>
       <c r="C46" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -1445,7 +3390,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -1456,7 +3401,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1467,7 +3412,7 @@
         <v>10</v>
       </c>
       <c r="C49" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1478,7 +3423,7 @@
         <v>11</v>
       </c>
       <c r="C50" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1489,7 +3434,7 @@
         <v>12</v>
       </c>
       <c r="C51" s="3">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D51" s="3">
         <f>C51-C38</f>
@@ -1504,7 +3449,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1515,7 +3460,7 @@
         <v>14</v>
       </c>
       <c r="C53" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1526,7 +3471,7 @@
         <v>15</v>
       </c>
       <c r="C54" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1537,7 +3482,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1548,7 +3493,7 @@
         <v>6</v>
       </c>
       <c r="C56" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1559,7 +3504,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1570,7 +3515,7 @@
         <v>8</v>
       </c>
       <c r="C58" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1581,7 +3526,7 @@
         <v>9</v>
       </c>
       <c r="C59" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1592,7 +3537,7 @@
         <v>10</v>
       </c>
       <c r="C60" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1603,7 +3548,7 @@
         <v>11</v>
       </c>
       <c r="C61" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1614,7 +3559,7 @@
         <v>12</v>
       </c>
       <c r="C62" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1625,7 +3570,7 @@
         <v>13</v>
       </c>
       <c r="C63" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D63" s="3">
         <f>C63-C51</f>
@@ -1640,7 +3585,7 @@
         <v>14</v>
       </c>
       <c r="C64" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1651,7 +3596,7 @@
         <v>15</v>
       </c>
       <c r="C65" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1662,7 +3607,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1673,7 +3618,7 @@
         <v>7</v>
       </c>
       <c r="C67" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1684,7 +3629,7 @@
         <v>8</v>
       </c>
       <c r="C68" s="1">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1695,7 +3640,7 @@
         <v>9</v>
       </c>
       <c r="C69" s="1">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1706,7 +3651,7 @@
         <v>10</v>
       </c>
       <c r="C70" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1717,7 +3662,7 @@
         <v>11</v>
       </c>
       <c r="C71" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1728,7 +3673,7 @@
         <v>12</v>
       </c>
       <c r="C72" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1739,7 +3684,7 @@
         <v>13</v>
       </c>
       <c r="C73" s="2">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1750,7 +3695,7 @@
         <v>14</v>
       </c>
       <c r="C74" s="3">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D74" s="1">
         <f>C74-C63</f>
@@ -1765,7 +3710,7 @@
         <v>15</v>
       </c>
       <c r="C75" s="1">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1776,7 +3721,7 @@
         <v>16</v>
       </c>
       <c r="C76" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -1787,7 +3732,7 @@
         <v>8</v>
       </c>
       <c r="C77" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1798,7 +3743,7 @@
         <v>9</v>
       </c>
       <c r="C78" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1809,7 +3754,7 @@
         <v>10</v>
       </c>
       <c r="C79" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1820,7 +3765,7 @@
         <v>11</v>
       </c>
       <c r="C80" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1831,7 +3776,7 @@
         <v>12</v>
       </c>
       <c r="C81" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1842,7 +3787,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1853,7 +3798,7 @@
         <v>14</v>
       </c>
       <c r="C83" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -1864,7 +3809,7 @@
         <v>15</v>
       </c>
       <c r="C84" s="3">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D84" s="1">
         <f>C84-C74</f>
@@ -1879,7 +3824,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1890,7 +3835,7 @@
         <v>9</v>
       </c>
       <c r="C86" s="1">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -1901,7 +3846,7 @@
         <v>10</v>
       </c>
       <c r="C87" s="1">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -1912,7 +3857,7 @@
         <v>11</v>
       </c>
       <c r="C88" s="1">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -1923,7 +3868,7 @@
         <v>12</v>
       </c>
       <c r="C89" s="1">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -1934,7 +3879,7 @@
         <v>13</v>
       </c>
       <c r="C90" s="1">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -1945,7 +3890,7 @@
         <v>14</v>
       </c>
       <c r="C91" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,7 +3901,7 @@
         <v>15</v>
       </c>
       <c r="C92" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -1967,7 +3912,7 @@
         <v>16</v>
       </c>
       <c r="C93" s="3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D93" s="1">
         <f>C93-C84</f>

</xml_diff>

<commit_message>
Testing 3rd Order Polynomials
</commit_message>
<xml_diff>
--- a/FilteredElectrodesPairs.xlsx
+++ b/FilteredElectrodesPairs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekty\rocsoledataconverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87AAC2E-BE6C-45F2-BE72-BC084C7449DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E28ABD5-C651-4E23-9F28-EF6833907E4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="2" r:id="rId1"/>
-    <sheet name="Normalized" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Normalized" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -410,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F37C97E-4A92-48F8-8517-257DD2D99655}">
-  <dimension ref="A1:O137"/>
+  <dimension ref="A1:Q257"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>8</v>
       </c>
@@ -430,7 +431,7 @@
         <v>Matlab 1-based without VoltageStamps</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -447,7 +448,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="s">
         <v>0</v>
@@ -456,7 +457,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -473,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -486,7 +487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -503,13 +504,13 @@
         <v>3</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -526,7 +527,7 @@
         <v>4</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -535,7 +536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -553,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I6">
         <v>4</v>
@@ -569,8 +570,11 @@
         <f>N2/2</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -587,7 +591,7 @@
         <v>6</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I7">
         <v>5</v>
@@ -603,8 +607,11 @@
         <f>IF(M6&gt;=$N$3,"",O6+$N$2)</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -621,7 +628,7 @@
         <v>7</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8">
         <v>6</v>
@@ -637,8 +644,11 @@
         <f t="shared" ref="O8:O26" si="1">IF(M7&gt;=$N$3,"",O7+$N$2)</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -655,7 +665,7 @@
         <v>8</v>
       </c>
       <c r="H9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I9">
         <v>7</v>
@@ -671,8 +681,11 @@
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -689,7 +702,7 @@
         <v>9</v>
       </c>
       <c r="H10" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I10" s="6">
         <v>8</v>
@@ -706,8 +719,11 @@
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q10">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -724,7 +740,7 @@
         <v>10</v>
       </c>
       <c r="H11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I11">
         <v>9</v>
@@ -740,8 +756,11 @@
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q11">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -758,7 +777,7 @@
         <v>11</v>
       </c>
       <c r="H12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I12">
         <v>10</v>
@@ -774,8 +793,11 @@
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -792,7 +814,7 @@
         <v>12</v>
       </c>
       <c r="H13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I13">
         <v>11</v>
@@ -808,8 +830,11 @@
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q13">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -826,7 +851,7 @@
         <v>13</v>
       </c>
       <c r="H14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I14">
         <v>12</v>
@@ -834,16 +859,18 @@
       <c r="M14">
         <v>9</v>
       </c>
-      <c r="N14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N14">
+        <v>129</v>
       </c>
       <c r="O14" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q14">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>2</v>
       </c>
@@ -864,7 +891,7 @@
         <v>14</v>
       </c>
       <c r="H15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I15">
         <v>13</v>
@@ -872,16 +899,18 @@
       <c r="M15">
         <v>10</v>
       </c>
-      <c r="N15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N15">
+        <v>146</v>
       </c>
       <c r="O15" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q15">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -898,7 +927,7 @@
         <v>15</v>
       </c>
       <c r="H16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I16">
         <v>14</v>
@@ -906,16 +935,18 @@
       <c r="M16">
         <v>11</v>
       </c>
-      <c r="N16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N16">
+        <v>163</v>
       </c>
       <c r="O16" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q16">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -932,7 +963,7 @@
         <v>16</v>
       </c>
       <c r="H17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I17">
         <v>15</v>
@@ -940,16 +971,18 @@
       <c r="M17">
         <v>12</v>
       </c>
-      <c r="N17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N17">
+        <v>180</v>
       </c>
       <c r="O17" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q17">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -966,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I18">
         <v>16</v>
@@ -974,16 +1007,15 @@
       <c r="M18">
         <v>13</v>
       </c>
-      <c r="N18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N18">
+        <v>197</v>
       </c>
       <c r="O18" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1000,21 +1032,20 @@
         <v>2</v>
       </c>
       <c r="H19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M19">
         <v>14</v>
       </c>
-      <c r="N19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N19">
+        <v>214</v>
       </c>
       <c r="O19" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1031,7 +1062,7 @@
         <v>3</v>
       </c>
       <c r="H20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I20">
         <v>17</v>
@@ -1039,16 +1070,15 @@
       <c r="M20">
         <v>15</v>
       </c>
-      <c r="N20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N20">
+        <v>231</v>
       </c>
       <c r="O20" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1065,7 +1095,7 @@
         <v>4</v>
       </c>
       <c r="H21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I21">
         <v>18</v>
@@ -1073,16 +1103,15 @@
       <c r="M21">
         <v>16</v>
       </c>
-      <c r="N21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="N21">
+        <v>248</v>
       </c>
       <c r="O21" s="2" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1099,7 +1128,7 @@
         <v>5</v>
       </c>
       <c r="H22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I22">
         <v>19</v>
@@ -1116,7 +1145,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1133,7 +1162,7 @@
         <v>6</v>
       </c>
       <c r="H23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I23">
         <v>20</v>
@@ -1150,7 +1179,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>3</v>
       </c>
@@ -1171,7 +1200,7 @@
         <v>7</v>
       </c>
       <c r="H24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I24">
         <v>21</v>
@@ -1188,7 +1217,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1205,7 +1234,7 @@
         <v>8</v>
       </c>
       <c r="H25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I25">
         <v>22</v>
@@ -1222,7 +1251,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
@@ -1239,7 +1268,7 @@
         <v>9</v>
       </c>
       <c r="H26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I26">
         <v>23</v>
@@ -1256,7 +1285,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1273,7 +1302,7 @@
         <v>10</v>
       </c>
       <c r="H27" s="6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I27" s="6">
         <v>24</v>
@@ -1283,7 +1312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1300,13 +1329,13 @@
         <v>11</v>
       </c>
       <c r="H28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I28" s="9">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1323,13 +1352,13 @@
         <v>12</v>
       </c>
       <c r="H29">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1346,13 +1375,13 @@
         <v>13</v>
       </c>
       <c r="H30">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I30">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1369,13 +1398,13 @@
         <v>14</v>
       </c>
       <c r="H31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I31">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1392,7 +1421,7 @@
         <v>15</v>
       </c>
       <c r="H32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I32">
         <v>29</v>
@@ -1419,7 +1448,7 @@
         <v>16</v>
       </c>
       <c r="H33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I33">
         <v>30</v>
@@ -1433,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="H34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I34">
         <v>31</v>
@@ -1447,7 +1476,7 @@
         <v>2</v>
       </c>
       <c r="H35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I35">
         <v>32</v>
@@ -1461,7 +1490,7 @@
         <v>3</v>
       </c>
       <c r="H36">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -1472,7 +1501,7 @@
         <v>4</v>
       </c>
       <c r="H37">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I37" s="10">
         <v>33</v>
@@ -1486,7 +1515,7 @@
         <v>5</v>
       </c>
       <c r="H38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I38" s="10">
         <v>34</v>
@@ -1500,7 +1529,7 @@
         <v>6</v>
       </c>
       <c r="H39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I39" s="10">
         <v>35</v>
@@ -1514,7 +1543,7 @@
         <v>7</v>
       </c>
       <c r="H40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I40" s="10">
         <v>36</v>
@@ -1528,7 +1557,7 @@
         <v>8</v>
       </c>
       <c r="H41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I41" s="10">
         <v>37</v>
@@ -1542,7 +1571,7 @@
         <v>9</v>
       </c>
       <c r="H42">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I42" s="10">
         <v>38</v>
@@ -1556,7 +1585,7 @@
         <v>10</v>
       </c>
       <c r="H43">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I43" s="10">
         <v>39</v>
@@ -1570,7 +1599,7 @@
         <v>11</v>
       </c>
       <c r="H44" s="6">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I44" s="6">
         <v>40</v>
@@ -1588,7 +1617,7 @@
         <v>12</v>
       </c>
       <c r="H45">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I45" s="10">
         <v>41</v>
@@ -1602,7 +1631,7 @@
         <v>13</v>
       </c>
       <c r="H46">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I46" s="10">
         <v>42</v>
@@ -1616,7 +1645,7 @@
         <v>14</v>
       </c>
       <c r="H47">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I47" s="10">
         <v>43</v>
@@ -1630,7 +1659,7 @@
         <v>15</v>
       </c>
       <c r="H48">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I48" s="10">
         <v>44</v>
@@ -1644,7 +1673,7 @@
         <v>16</v>
       </c>
       <c r="H49">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I49" s="10">
         <v>45</v>
@@ -1658,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="H50">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I50" s="10">
         <v>46</v>
@@ -1672,7 +1701,7 @@
         <v>2</v>
       </c>
       <c r="H51">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I51" s="10">
         <v>47</v>
@@ -1686,7 +1715,7 @@
         <v>3</v>
       </c>
       <c r="H52">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I52" s="10">
         <v>48</v>
@@ -1700,7 +1729,7 @@
         <v>4</v>
       </c>
       <c r="H53">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I53" s="10"/>
     </row>
@@ -1712,7 +1741,7 @@
         <v>5</v>
       </c>
       <c r="H54">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I54" s="10">
         <v>49</v>
@@ -1726,7 +1755,7 @@
         <v>6</v>
       </c>
       <c r="H55">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I55" s="10">
         <v>50</v>
@@ -1740,7 +1769,7 @@
         <v>7</v>
       </c>
       <c r="H56">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I56" s="10">
         <v>51</v>
@@ -1754,7 +1783,7 @@
         <v>8</v>
       </c>
       <c r="H57">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I57" s="10">
         <v>52</v>
@@ -1768,7 +1797,7 @@
         <v>9</v>
       </c>
       <c r="H58">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I58" s="10">
         <v>53</v>
@@ -1782,7 +1811,7 @@
         <v>10</v>
       </c>
       <c r="H59">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I59" s="10">
         <v>54</v>
@@ -1796,7 +1825,7 @@
         <v>11</v>
       </c>
       <c r="H60">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I60" s="10">
         <v>55</v>
@@ -1810,7 +1839,7 @@
         <v>12</v>
       </c>
       <c r="H61" s="6">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I61" s="6">
         <v>56</v>
@@ -1828,7 +1857,7 @@
         <v>13</v>
       </c>
       <c r="H62">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I62" s="10">
         <v>57</v>
@@ -1842,7 +1871,7 @@
         <v>14</v>
       </c>
       <c r="H63">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I63" s="10">
         <v>58</v>
@@ -1856,7 +1885,7 @@
         <v>15</v>
       </c>
       <c r="H64">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I64" s="10">
         <v>59</v>
@@ -1870,7 +1899,7 @@
         <v>16</v>
       </c>
       <c r="H65">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I65" s="10">
         <v>60</v>
@@ -1884,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="H66">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I66" s="10">
         <v>61</v>
@@ -1898,7 +1927,7 @@
         <v>2</v>
       </c>
       <c r="H67">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I67" s="10">
         <v>62</v>
@@ -1912,7 +1941,7 @@
         <v>3</v>
       </c>
       <c r="H68">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I68" s="10">
         <v>63</v>
@@ -1926,7 +1955,7 @@
         <v>4</v>
       </c>
       <c r="H69">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I69" s="10">
         <v>64</v>
@@ -1940,7 +1969,7 @@
         <v>5</v>
       </c>
       <c r="H70">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I70" s="10">
         <v>65</v>
@@ -1954,7 +1983,7 @@
         <v>6</v>
       </c>
       <c r="H71">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I71" s="10"/>
     </row>
@@ -1966,7 +1995,7 @@
         <v>7</v>
       </c>
       <c r="H72">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I72" s="10">
         <v>66</v>
@@ -1980,7 +2009,7 @@
         <v>8</v>
       </c>
       <c r="H73">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I73" s="10">
         <v>67</v>
@@ -1994,7 +2023,7 @@
         <v>9</v>
       </c>
       <c r="H74">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I74" s="10">
         <v>68</v>
@@ -2008,7 +2037,7 @@
         <v>10</v>
       </c>
       <c r="H75">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I75" s="10">
         <v>69</v>
@@ -2022,7 +2051,7 @@
         <v>11</v>
       </c>
       <c r="H76">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I76" s="10">
         <v>70</v>
@@ -2036,7 +2065,7 @@
         <v>12</v>
       </c>
       <c r="H77">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I77" s="10">
         <v>71</v>
@@ -2050,7 +2079,7 @@
         <v>13</v>
       </c>
       <c r="H78" s="6">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I78" s="6">
         <v>72</v>
@@ -2068,7 +2097,7 @@
         <v>14</v>
       </c>
       <c r="H79">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I79" s="10">
         <v>73</v>
@@ -2082,7 +2111,7 @@
         <v>15</v>
       </c>
       <c r="H80">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I80" s="10">
         <v>74</v>
@@ -2096,7 +2125,7 @@
         <v>16</v>
       </c>
       <c r="H81">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I81" s="10">
         <v>75</v>
@@ -2110,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="H82">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I82" s="10">
         <v>76</v>
@@ -2124,7 +2153,7 @@
         <v>2</v>
       </c>
       <c r="H83">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I83" s="10">
         <v>77</v>
@@ -2138,7 +2167,7 @@
         <v>3</v>
       </c>
       <c r="H84">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I84" s="10">
         <v>78</v>
@@ -2152,7 +2181,7 @@
         <v>4</v>
       </c>
       <c r="H85">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I85" s="10">
         <v>79</v>
@@ -2166,7 +2195,7 @@
         <v>5</v>
       </c>
       <c r="H86">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I86" s="10">
         <v>80</v>
@@ -2180,7 +2209,7 @@
         <v>6</v>
       </c>
       <c r="H87">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I87" s="10">
         <v>81</v>
@@ -2194,7 +2223,7 @@
         <v>7</v>
       </c>
       <c r="H88">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I88" s="10"/>
     </row>
@@ -2206,7 +2235,7 @@
         <v>8</v>
       </c>
       <c r="H89">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I89" s="10">
         <v>82</v>
@@ -2220,7 +2249,7 @@
         <v>9</v>
       </c>
       <c r="H90">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I90" s="10">
         <v>83</v>
@@ -2234,7 +2263,7 @@
         <v>10</v>
       </c>
       <c r="H91">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I91" s="10">
         <v>84</v>
@@ -2248,7 +2277,7 @@
         <v>11</v>
       </c>
       <c r="H92">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I92" s="10">
         <v>85</v>
@@ -2262,7 +2291,7 @@
         <v>12</v>
       </c>
       <c r="H93">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I93" s="10">
         <v>86</v>
@@ -2276,7 +2305,7 @@
         <v>13</v>
       </c>
       <c r="H94">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I94" s="10">
         <v>87</v>
@@ -2290,7 +2319,7 @@
         <v>14</v>
       </c>
       <c r="H95" s="6">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I95" s="6">
         <v>88</v>
@@ -2308,7 +2337,7 @@
         <v>15</v>
       </c>
       <c r="H96">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I96" s="10">
         <v>89</v>
@@ -2322,7 +2351,7 @@
         <v>16</v>
       </c>
       <c r="H97">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I97" s="10">
         <v>90</v>
@@ -2336,7 +2365,7 @@
         <v>1</v>
       </c>
       <c r="H98">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I98" s="10">
         <v>91</v>
@@ -2350,7 +2379,7 @@
         <v>2</v>
       </c>
       <c r="H99">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I99" s="10">
         <v>92</v>
@@ -2364,7 +2393,7 @@
         <v>3</v>
       </c>
       <c r="H100">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I100" s="10">
         <v>93</v>
@@ -2378,7 +2407,7 @@
         <v>4</v>
       </c>
       <c r="H101">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I101" s="10">
         <v>94</v>
@@ -2392,7 +2421,7 @@
         <v>5</v>
       </c>
       <c r="H102">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I102" s="10">
         <v>95</v>
@@ -2406,7 +2435,7 @@
         <v>6</v>
       </c>
       <c r="H103">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I103" s="10">
         <v>96</v>
@@ -2420,7 +2449,7 @@
         <v>7</v>
       </c>
       <c r="H104">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I104" s="10">
         <v>97</v>
@@ -2434,7 +2463,7 @@
         <v>8</v>
       </c>
       <c r="H105">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I105" s="10"/>
     </row>
@@ -2446,7 +2475,7 @@
         <v>9</v>
       </c>
       <c r="H106">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I106" s="10">
         <v>98</v>
@@ -2460,7 +2489,7 @@
         <v>10</v>
       </c>
       <c r="H107">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I107" s="10">
         <v>99</v>
@@ -2474,7 +2503,7 @@
         <v>11</v>
       </c>
       <c r="H108">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I108" s="10">
         <v>100</v>
@@ -2488,7 +2517,7 @@
         <v>12</v>
       </c>
       <c r="H109">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I109" s="10">
         <v>101</v>
@@ -2502,7 +2531,7 @@
         <v>13</v>
       </c>
       <c r="H110">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I110" s="10">
         <v>102</v>
@@ -2516,7 +2545,7 @@
         <v>14</v>
       </c>
       <c r="H111">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I111" s="10">
         <v>103</v>
@@ -2530,7 +2559,7 @@
         <v>15</v>
       </c>
       <c r="H112" s="6">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I112" s="6">
         <v>104</v>
@@ -2548,7 +2577,7 @@
         <v>16</v>
       </c>
       <c r="H113">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I113" s="10">
         <v>105</v>
@@ -2562,7 +2591,7 @@
         <v>1</v>
       </c>
       <c r="H114">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I114" s="10">
         <v>106</v>
@@ -2576,7 +2605,7 @@
         <v>2</v>
       </c>
       <c r="H115">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I115" s="10">
         <v>107</v>
@@ -2590,7 +2619,7 @@
         <v>3</v>
       </c>
       <c r="H116">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I116" s="10">
         <v>108</v>
@@ -2604,7 +2633,7 @@
         <v>4</v>
       </c>
       <c r="H117">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I117" s="10">
         <v>109</v>
@@ -2618,7 +2647,7 @@
         <v>5</v>
       </c>
       <c r="H118">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I118" s="10">
         <v>110</v>
@@ -2632,7 +2661,7 @@
         <v>6</v>
       </c>
       <c r="H119">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I119" s="10">
         <v>111</v>
@@ -2646,7 +2675,7 @@
         <v>7</v>
       </c>
       <c r="H120">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I120" s="10">
         <v>112</v>
@@ -2660,7 +2689,7 @@
         <v>8</v>
       </c>
       <c r="H121">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I121" s="10">
         <v>113</v>
@@ -2674,7 +2703,7 @@
         <v>9</v>
       </c>
       <c r="H122">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I122" s="10"/>
     </row>
@@ -2686,7 +2715,7 @@
         <v>10</v>
       </c>
       <c r="H123">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I123" s="10">
         <v>114</v>
@@ -2700,7 +2729,7 @@
         <v>11</v>
       </c>
       <c r="H124">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I124" s="10">
         <v>115</v>
@@ -2714,7 +2743,7 @@
         <v>12</v>
       </c>
       <c r="H125">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I125" s="10">
         <v>116</v>
@@ -2728,7 +2757,7 @@
         <v>13</v>
       </c>
       <c r="H126">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I126" s="10">
         <v>117</v>
@@ -2742,7 +2771,7 @@
         <v>14</v>
       </c>
       <c r="H127">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I127" s="10">
         <v>118</v>
@@ -2756,7 +2785,7 @@
         <v>15</v>
       </c>
       <c r="H128">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I128" s="10">
         <v>119</v>
@@ -2770,7 +2799,7 @@
         <v>16</v>
       </c>
       <c r="H129" s="6">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I129" s="6">
         <v>120</v>
@@ -2781,35 +2810,1440 @@
       </c>
     </row>
     <row r="130" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F130" s="6">
+        <v>9</v>
+      </c>
+      <c r="G130" s="6">
+        <v>1</v>
+      </c>
+      <c r="H130" s="6">
+        <v>129</v>
+      </c>
       <c r="I130" s="10"/>
     </row>
     <row r="131" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F131">
+        <v>9</v>
+      </c>
+      <c r="G131">
+        <v>2</v>
+      </c>
+      <c r="H131">
+        <v>130</v>
+      </c>
       <c r="I131" s="10"/>
     </row>
     <row r="132" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F132">
+        <v>9</v>
+      </c>
+      <c r="G132">
+        <v>3</v>
+      </c>
+      <c r="H132">
+        <v>131</v>
+      </c>
       <c r="I132" s="10"/>
     </row>
     <row r="133" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F133" s="10">
+        <v>9</v>
+      </c>
+      <c r="G133" s="10">
+        <v>4</v>
+      </c>
+      <c r="H133" s="10">
+        <v>132</v>
+      </c>
       <c r="I133" s="10"/>
     </row>
     <row r="134" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F134">
+        <v>9</v>
+      </c>
+      <c r="G134">
+        <v>5</v>
+      </c>
+      <c r="H134">
+        <v>133</v>
+      </c>
       <c r="I134" s="10"/>
     </row>
     <row r="135" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F135">
+        <v>9</v>
+      </c>
+      <c r="G135">
+        <v>6</v>
+      </c>
+      <c r="H135">
+        <v>134</v>
+      </c>
       <c r="I135" s="10"/>
     </row>
     <row r="136" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F136">
+        <v>9</v>
+      </c>
+      <c r="G136">
+        <v>7</v>
+      </c>
+      <c r="H136">
+        <v>135</v>
+      </c>
       <c r="I136" s="10"/>
     </row>
     <row r="137" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F137">
+        <v>9</v>
+      </c>
+      <c r="G137">
+        <v>8</v>
+      </c>
+      <c r="H137" s="10">
+        <v>136</v>
+      </c>
       <c r="I137" s="10"/>
     </row>
+    <row r="138" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F138" s="8">
+        <v>9</v>
+      </c>
+      <c r="G138" s="8">
+        <v>9</v>
+      </c>
+      <c r="H138" s="10">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F139">
+        <v>9</v>
+      </c>
+      <c r="G139">
+        <v>10</v>
+      </c>
+      <c r="H139" s="10">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F140">
+        <v>9</v>
+      </c>
+      <c r="G140">
+        <v>11</v>
+      </c>
+      <c r="H140" s="10">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F141">
+        <v>9</v>
+      </c>
+      <c r="G141">
+        <v>12</v>
+      </c>
+      <c r="H141" s="10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F142">
+        <v>9</v>
+      </c>
+      <c r="G142">
+        <v>13</v>
+      </c>
+      <c r="H142" s="10">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F143">
+        <v>9</v>
+      </c>
+      <c r="G143">
+        <v>14</v>
+      </c>
+      <c r="H143" s="10">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F144">
+        <v>9</v>
+      </c>
+      <c r="G144">
+        <v>15</v>
+      </c>
+      <c r="H144" s="10">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F145">
+        <v>9</v>
+      </c>
+      <c r="G145">
+        <v>16</v>
+      </c>
+      <c r="H145" s="10">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F146">
+        <v>10</v>
+      </c>
+      <c r="G146">
+        <v>1</v>
+      </c>
+      <c r="H146" s="10">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F147" s="6">
+        <v>10</v>
+      </c>
+      <c r="G147" s="6">
+        <v>2</v>
+      </c>
+      <c r="H147" s="6">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F148">
+        <v>10</v>
+      </c>
+      <c r="G148">
+        <v>3</v>
+      </c>
+      <c r="H148" s="10">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F149">
+        <v>10</v>
+      </c>
+      <c r="G149">
+        <v>4</v>
+      </c>
+      <c r="H149" s="10">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F150">
+        <v>10</v>
+      </c>
+      <c r="G150">
+        <v>5</v>
+      </c>
+      <c r="H150" s="10">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F151">
+        <v>10</v>
+      </c>
+      <c r="G151">
+        <v>6</v>
+      </c>
+      <c r="H151" s="10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F152">
+        <v>10</v>
+      </c>
+      <c r="G152">
+        <v>7</v>
+      </c>
+      <c r="H152" s="10">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F153">
+        <v>10</v>
+      </c>
+      <c r="G153">
+        <v>8</v>
+      </c>
+      <c r="H153" s="10">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F154">
+        <v>10</v>
+      </c>
+      <c r="G154">
+        <v>9</v>
+      </c>
+      <c r="H154" s="10">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F155" s="8">
+        <v>10</v>
+      </c>
+      <c r="G155" s="8">
+        <v>10</v>
+      </c>
+      <c r="H155" s="10">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F156">
+        <v>10</v>
+      </c>
+      <c r="G156">
+        <v>11</v>
+      </c>
+      <c r="H156" s="10">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F157">
+        <v>10</v>
+      </c>
+      <c r="G157">
+        <v>12</v>
+      </c>
+      <c r="H157" s="10">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F158">
+        <v>10</v>
+      </c>
+      <c r="G158">
+        <v>13</v>
+      </c>
+      <c r="H158" s="10">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F159">
+        <v>10</v>
+      </c>
+      <c r="G159">
+        <v>14</v>
+      </c>
+      <c r="H159" s="10">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F160">
+        <v>10</v>
+      </c>
+      <c r="G160">
+        <v>15</v>
+      </c>
+      <c r="H160" s="10">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F161">
+        <v>10</v>
+      </c>
+      <c r="G161">
+        <v>16</v>
+      </c>
+      <c r="H161" s="10">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F162">
+        <v>11</v>
+      </c>
+      <c r="G162">
+        <v>1</v>
+      </c>
+      <c r="H162" s="10">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F163">
+        <v>11</v>
+      </c>
+      <c r="G163">
+        <v>2</v>
+      </c>
+      <c r="H163" s="10">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F164" s="6">
+        <v>11</v>
+      </c>
+      <c r="G164" s="6">
+        <v>3</v>
+      </c>
+      <c r="H164" s="6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F165">
+        <v>11</v>
+      </c>
+      <c r="G165">
+        <v>4</v>
+      </c>
+      <c r="H165" s="10">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F166">
+        <v>11</v>
+      </c>
+      <c r="G166">
+        <v>5</v>
+      </c>
+      <c r="H166" s="10">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F167">
+        <v>11</v>
+      </c>
+      <c r="G167">
+        <v>6</v>
+      </c>
+      <c r="H167" s="10">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F168">
+        <v>11</v>
+      </c>
+      <c r="G168">
+        <v>7</v>
+      </c>
+      <c r="H168" s="10">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F169">
+        <v>11</v>
+      </c>
+      <c r="G169">
+        <v>8</v>
+      </c>
+      <c r="H169" s="10">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F170">
+        <v>11</v>
+      </c>
+      <c r="G170">
+        <v>9</v>
+      </c>
+      <c r="H170" s="10">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F171">
+        <v>11</v>
+      </c>
+      <c r="G171">
+        <v>10</v>
+      </c>
+      <c r="H171" s="10">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F172">
+        <v>11</v>
+      </c>
+      <c r="G172">
+        <v>11</v>
+      </c>
+      <c r="H172" s="10">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F173">
+        <v>11</v>
+      </c>
+      <c r="G173">
+        <v>12</v>
+      </c>
+      <c r="H173" s="10">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F174">
+        <v>11</v>
+      </c>
+      <c r="G174">
+        <v>13</v>
+      </c>
+      <c r="H174" s="10">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F175">
+        <v>11</v>
+      </c>
+      <c r="G175">
+        <v>14</v>
+      </c>
+      <c r="H175" s="10">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F176">
+        <v>11</v>
+      </c>
+      <c r="G176">
+        <v>15</v>
+      </c>
+      <c r="H176" s="10">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F177">
+        <v>11</v>
+      </c>
+      <c r="G177">
+        <v>16</v>
+      </c>
+      <c r="H177" s="10">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F178">
+        <v>12</v>
+      </c>
+      <c r="G178">
+        <v>1</v>
+      </c>
+      <c r="H178" s="10">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F179">
+        <v>12</v>
+      </c>
+      <c r="G179">
+        <v>2</v>
+      </c>
+      <c r="H179" s="10">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F180">
+        <v>12</v>
+      </c>
+      <c r="G180">
+        <v>3</v>
+      </c>
+      <c r="H180" s="10">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F181" s="6">
+        <v>12</v>
+      </c>
+      <c r="G181" s="6">
+        <v>4</v>
+      </c>
+      <c r="H181" s="6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F182">
+        <v>12</v>
+      </c>
+      <c r="G182">
+        <v>5</v>
+      </c>
+      <c r="H182" s="10">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F183">
+        <v>12</v>
+      </c>
+      <c r="G183">
+        <v>6</v>
+      </c>
+      <c r="H183" s="10">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F184">
+        <v>12</v>
+      </c>
+      <c r="G184">
+        <v>7</v>
+      </c>
+      <c r="H184" s="10">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F185">
+        <v>12</v>
+      </c>
+      <c r="G185">
+        <v>8</v>
+      </c>
+      <c r="H185" s="10">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F186">
+        <v>12</v>
+      </c>
+      <c r="G186">
+        <v>9</v>
+      </c>
+      <c r="H186" s="10">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F187">
+        <v>12</v>
+      </c>
+      <c r="G187">
+        <v>10</v>
+      </c>
+      <c r="H187" s="10">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F188">
+        <v>12</v>
+      </c>
+      <c r="G188">
+        <v>11</v>
+      </c>
+      <c r="H188" s="10">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F189" s="8">
+        <v>12</v>
+      </c>
+      <c r="G189" s="8">
+        <v>12</v>
+      </c>
+      <c r="H189" s="10">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F190">
+        <v>12</v>
+      </c>
+      <c r="G190">
+        <v>13</v>
+      </c>
+      <c r="H190" s="10">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F191">
+        <v>12</v>
+      </c>
+      <c r="G191">
+        <v>14</v>
+      </c>
+      <c r="H191" s="10">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F192">
+        <v>12</v>
+      </c>
+      <c r="G192">
+        <v>15</v>
+      </c>
+      <c r="H192" s="10">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F193">
+        <v>12</v>
+      </c>
+      <c r="G193">
+        <v>16</v>
+      </c>
+      <c r="H193" s="10">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F194">
+        <v>13</v>
+      </c>
+      <c r="G194">
+        <v>1</v>
+      </c>
+      <c r="H194" s="10">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F195">
+        <v>13</v>
+      </c>
+      <c r="G195">
+        <v>2</v>
+      </c>
+      <c r="H195" s="10">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F196">
+        <v>13</v>
+      </c>
+      <c r="G196">
+        <v>3</v>
+      </c>
+      <c r="H196" s="10">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F197">
+        <v>13</v>
+      </c>
+      <c r="G197">
+        <v>4</v>
+      </c>
+      <c r="H197" s="10">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F198" s="6">
+        <v>13</v>
+      </c>
+      <c r="G198" s="6">
+        <v>5</v>
+      </c>
+      <c r="H198" s="6">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F199">
+        <v>13</v>
+      </c>
+      <c r="G199">
+        <v>6</v>
+      </c>
+      <c r="H199" s="10">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F200">
+        <v>13</v>
+      </c>
+      <c r="G200">
+        <v>7</v>
+      </c>
+      <c r="H200" s="10">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F201">
+        <v>13</v>
+      </c>
+      <c r="G201">
+        <v>8</v>
+      </c>
+      <c r="H201" s="10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F202">
+        <v>13</v>
+      </c>
+      <c r="G202">
+        <v>9</v>
+      </c>
+      <c r="H202" s="10">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F203">
+        <v>13</v>
+      </c>
+      <c r="G203">
+        <v>10</v>
+      </c>
+      <c r="H203" s="10">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F204">
+        <v>13</v>
+      </c>
+      <c r="G204">
+        <v>11</v>
+      </c>
+      <c r="H204" s="10">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F205">
+        <v>13</v>
+      </c>
+      <c r="G205">
+        <v>12</v>
+      </c>
+      <c r="H205" s="10">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F206" s="8">
+        <v>13</v>
+      </c>
+      <c r="G206" s="8">
+        <v>13</v>
+      </c>
+      <c r="H206" s="10">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F207">
+        <v>13</v>
+      </c>
+      <c r="G207">
+        <v>14</v>
+      </c>
+      <c r="H207" s="10">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F208">
+        <v>13</v>
+      </c>
+      <c r="G208">
+        <v>15</v>
+      </c>
+      <c r="H208" s="10">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F209">
+        <v>13</v>
+      </c>
+      <c r="G209">
+        <v>16</v>
+      </c>
+      <c r="H209" s="10">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F210">
+        <v>14</v>
+      </c>
+      <c r="G210">
+        <v>1</v>
+      </c>
+      <c r="H210" s="10">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F211">
+        <v>14</v>
+      </c>
+      <c r="G211">
+        <v>2</v>
+      </c>
+      <c r="H211" s="10">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F212">
+        <v>14</v>
+      </c>
+      <c r="G212">
+        <v>3</v>
+      </c>
+      <c r="H212" s="10">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F213">
+        <v>14</v>
+      </c>
+      <c r="G213">
+        <v>4</v>
+      </c>
+      <c r="H213" s="10">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F214">
+        <v>14</v>
+      </c>
+      <c r="G214">
+        <v>5</v>
+      </c>
+      <c r="H214" s="10">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F215" s="6">
+        <v>14</v>
+      </c>
+      <c r="G215" s="6">
+        <v>6</v>
+      </c>
+      <c r="H215" s="6">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F216">
+        <v>14</v>
+      </c>
+      <c r="G216">
+        <v>7</v>
+      </c>
+      <c r="H216" s="10">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F217">
+        <v>14</v>
+      </c>
+      <c r="G217">
+        <v>8</v>
+      </c>
+      <c r="H217" s="10">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F218">
+        <v>14</v>
+      </c>
+      <c r="G218">
+        <v>9</v>
+      </c>
+      <c r="H218" s="10">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F219">
+        <v>14</v>
+      </c>
+      <c r="G219">
+        <v>10</v>
+      </c>
+      <c r="H219" s="10">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F220">
+        <v>14</v>
+      </c>
+      <c r="G220">
+        <v>11</v>
+      </c>
+      <c r="H220" s="10">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F221">
+        <v>14</v>
+      </c>
+      <c r="G221">
+        <v>12</v>
+      </c>
+      <c r="H221" s="10">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F222">
+        <v>14</v>
+      </c>
+      <c r="G222">
+        <v>13</v>
+      </c>
+      <c r="H222" s="10">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F223" s="8">
+        <v>14</v>
+      </c>
+      <c r="G223" s="8">
+        <v>14</v>
+      </c>
+      <c r="H223" s="8">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F224">
+        <v>14</v>
+      </c>
+      <c r="G224">
+        <v>15</v>
+      </c>
+      <c r="H224" s="10">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F225">
+        <v>14</v>
+      </c>
+      <c r="G225">
+        <v>16</v>
+      </c>
+      <c r="H225" s="10">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F226">
+        <v>15</v>
+      </c>
+      <c r="G226">
+        <v>1</v>
+      </c>
+      <c r="H226" s="10">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F227">
+        <v>15</v>
+      </c>
+      <c r="G227">
+        <v>2</v>
+      </c>
+      <c r="H227" s="10">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F228">
+        <v>15</v>
+      </c>
+      <c r="G228">
+        <v>3</v>
+      </c>
+      <c r="H228" s="10">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F229">
+        <v>15</v>
+      </c>
+      <c r="G229">
+        <v>4</v>
+      </c>
+      <c r="H229" s="10">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F230">
+        <v>15</v>
+      </c>
+      <c r="G230">
+        <v>5</v>
+      </c>
+      <c r="H230" s="10">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F231">
+        <v>15</v>
+      </c>
+      <c r="G231">
+        <v>6</v>
+      </c>
+      <c r="H231" s="10">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F232" s="6">
+        <v>15</v>
+      </c>
+      <c r="G232" s="6">
+        <v>7</v>
+      </c>
+      <c r="H232" s="6">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F233">
+        <v>15</v>
+      </c>
+      <c r="G233">
+        <v>8</v>
+      </c>
+      <c r="H233" s="10">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F234">
+        <v>15</v>
+      </c>
+      <c r="G234">
+        <v>9</v>
+      </c>
+      <c r="H234" s="10">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F235">
+        <v>15</v>
+      </c>
+      <c r="G235">
+        <v>10</v>
+      </c>
+      <c r="H235" s="10">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F236">
+        <v>15</v>
+      </c>
+      <c r="G236">
+        <v>11</v>
+      </c>
+      <c r="H236" s="10">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F237">
+        <v>15</v>
+      </c>
+      <c r="G237">
+        <v>12</v>
+      </c>
+      <c r="H237" s="10">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F238">
+        <v>15</v>
+      </c>
+      <c r="G238">
+        <v>13</v>
+      </c>
+      <c r="H238" s="10">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F239">
+        <v>15</v>
+      </c>
+      <c r="G239">
+        <v>14</v>
+      </c>
+      <c r="H239" s="10">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F240" s="8">
+        <v>15</v>
+      </c>
+      <c r="G240" s="8">
+        <v>15</v>
+      </c>
+      <c r="H240" s="10">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F241">
+        <v>15</v>
+      </c>
+      <c r="G241">
+        <v>16</v>
+      </c>
+      <c r="H241" s="10">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F242">
+        <v>16</v>
+      </c>
+      <c r="G242">
+        <v>1</v>
+      </c>
+      <c r="H242" s="10">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F243">
+        <v>16</v>
+      </c>
+      <c r="G243">
+        <v>2</v>
+      </c>
+      <c r="H243" s="10">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F244">
+        <v>16</v>
+      </c>
+      <c r="G244">
+        <v>3</v>
+      </c>
+      <c r="H244" s="10">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F245">
+        <v>16</v>
+      </c>
+      <c r="G245">
+        <v>4</v>
+      </c>
+      <c r="H245" s="10">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F246">
+        <v>16</v>
+      </c>
+      <c r="G246">
+        <v>5</v>
+      </c>
+      <c r="H246" s="10">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F247">
+        <v>16</v>
+      </c>
+      <c r="G247">
+        <v>6</v>
+      </c>
+      <c r="H247" s="10">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F248">
+        <v>16</v>
+      </c>
+      <c r="G248">
+        <v>7</v>
+      </c>
+      <c r="H248" s="10">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F249" s="6">
+        <v>16</v>
+      </c>
+      <c r="G249" s="6">
+        <v>8</v>
+      </c>
+      <c r="H249" s="6">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F250">
+        <v>16</v>
+      </c>
+      <c r="G250">
+        <v>9</v>
+      </c>
+      <c r="H250" s="10">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F251">
+        <v>16</v>
+      </c>
+      <c r="G251">
+        <v>10</v>
+      </c>
+      <c r="H251" s="10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F252">
+        <v>16</v>
+      </c>
+      <c r="G252">
+        <v>11</v>
+      </c>
+      <c r="H252" s="10">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F253">
+        <v>16</v>
+      </c>
+      <c r="G253">
+        <v>12</v>
+      </c>
+      <c r="H253" s="10">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F254">
+        <v>16</v>
+      </c>
+      <c r="G254">
+        <v>13</v>
+      </c>
+      <c r="H254" s="10">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F255">
+        <v>16</v>
+      </c>
+      <c r="G255">
+        <v>14</v>
+      </c>
+      <c r="H255" s="10">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F256">
+        <v>16</v>
+      </c>
+      <c r="G256">
+        <v>15</v>
+      </c>
+      <c r="H256" s="10">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F257">
+        <v>16</v>
+      </c>
+      <c r="G257">
+        <v>16</v>
+      </c>
+      <c r="H257" s="10">
+        <v>256</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF6F45B-435A-48F0-B624-205E59A86CEB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P93"/>
   <sheetViews>

</xml_diff>